<commit_message>
Sửa lỗi nhập liệu.
</commit_message>
<xml_diff>
--- a/datasets/TuyenVN_2019.xlsx
+++ b/datasets/TuyenVN_2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\github.com\thachln\thachln.github.io.git\thachln.github.io\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{688A4355-C60E-43F6-BBFB-C159BA6E37BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A54419-7B99-42FC-8C8C-CC44DA239A77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13035" yWindow="3870" windowWidth="15765" windowHeight="11730" xr2:uid="{CEDE83EC-5A3B-45E8-BE00-7D2708259BB2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CEDE83EC-5A3B-45E8-BE00-7D2708259BB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -626,7 +626,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G25"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,7 +948,7 @@
         <v>1995</v>
       </c>
       <c r="E14" s="5">
-        <v>73</v>
+        <v>173</v>
       </c>
       <c r="F14" s="5">
         <v>65</v>

</xml_diff>